<commit_message>
Fix testdata Connect importer of elicitation forms
</commit_message>
<xml_diff>
--- a/test/StoryTree.IO.Test/test-data/DotFormExample.xlsx
+++ b/test/StoryTree.IO.Test/test-data/DotFormExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\storytree\test\StoryTree.IO.Test\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2C7BF8EB-CEF1-47E6-9F9D-5B58837C83DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8D20594C-369B-496E-BE11-EE8441DE964D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>DOT Formulier</t>
   </si>
@@ -28,9 +28,6 @@
     <t>DOT = Deskundigen Oordeel Toets op Maat</t>
   </si>
   <si>
-    <t>Gebeurtenis 3: AGK - HHNK</t>
-  </si>
-  <si>
     <t>Expert:</t>
   </si>
   <si>
@@ -122,13 +119,19 @@
   </si>
   <si>
     <t>Dit is een toelichting</t>
+  </si>
+  <si>
+    <t>Gebeurtenis:</t>
+  </si>
+  <si>
+    <t>AGK - HHNK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -142,6 +145,12 @@
       <b/>
       <sz val="16"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -217,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -229,10 +238,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,13 +559,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="4" customWidth="1"/>
     <col min="3" max="7" width="12" customWidth="1"/>
@@ -562,98 +574,99 @@
     <col min="10" max="11" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
       <c r="J2" s="1"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="C5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="C5" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="C8" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="5">
         <v>43406.922442210598</v>
       </c>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>8</v>
+      <c r="G11" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="C12" s="2">
         <v>1</v>
@@ -662,17 +675,17 @@
         <v>0.999</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>8</v>
+      <c r="G12" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="C13" s="3">
         <v>2</v>
@@ -681,17 +694,17 @@
         <v>0.99</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>8</v>
+      <c r="G13" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="C14" s="2">
         <v>3</v>
@@ -700,17 +713,17 @@
         <v>0.9</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>8</v>
+      <c r="G14" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="C15" s="3">
         <v>4</v>
@@ -719,17 +732,17 @@
         <v>0.5</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>8</v>
+      <c r="G15" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="C16" s="2">
         <v>5</v>
@@ -738,17 +751,17 @@
         <v>0.1</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>8</v>
+      <c r="G16" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="C17" s="3">
         <v>6</v>
@@ -757,17 +770,17 @@
         <v>0.01</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>8</v>
+      <c r="G17" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="C18" s="2">
         <v>7</v>
@@ -776,61 +789,61 @@
         <v>1E-3</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>8</v>
+      <c r="G18" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="C22" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="C23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="C24" s="2">
         <v>2.2999999999999998</v>
@@ -849,11 +862,11 @@
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="C25" s="3">
         <v>2.6</v>
@@ -872,11 +885,11 @@
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="C26" s="2">
         <v>2.9</v>
@@ -895,11 +908,11 @@
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="C27" s="3">
         <v>3.2</v>
@@ -918,11 +931,11 @@
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="C28" s="2">
         <v>3.5</v>
@@ -941,11 +954,11 @@
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="C29" s="3">
         <v>3.8</v>
@@ -964,47 +977,47 @@
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="C31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="C32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="I32" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I32" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="C33" s="2">
         <v>2.2999999999999998</v>
@@ -1023,11 +1036,11 @@
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="C34" s="3">
         <v>2.6</v>
@@ -1046,11 +1059,11 @@
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="C35" s="2">
         <v>2.9</v>
@@ -1069,11 +1082,11 @@
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="C36" s="3">
         <v>3.2</v>
@@ -1092,11 +1105,11 @@
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="C37" s="2">
         <v>3.5</v>
@@ -1115,11 +1128,11 @@
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
       <c r="C38" s="3">
         <v>3.8</v>
@@ -1138,15 +1151,15 @@
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -1158,17 +1171,18 @@
       <c r="J40" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
   </mergeCells>
   <dataValidations count="36">
     <dataValidation type="list" allowBlank="1" sqref="E24" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>